<commit_message>
cost plan as of 2023-12-08 - sizes are now one of 1, 2, 4, 8, 16 - added conversion to days added - added note regarding orientation - now includes the mandatory Work Packages regarding project management - now considers all semesters
</commit_message>
<xml_diff>
--- a/documents/cost_plan/drawing2story-cost_plan.xlsx
+++ b/documents/cost_plan/drawing2story-cost_plan.xlsx
@@ -3,23 +3,45 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Tabelle1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="drawing2story - cost plan - eff" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="I5LDhB2mcRSA1x4FmsEoMHPUFutdii7qPNgjzVatS5I="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
-  <si>
-    <t>drawing2story cost plan - estimation of required work hours</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="113">
+  <si>
+    <t>drawing2story - cost plan - effort estimation</t>
   </si>
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>Functional Area (FA) - Work Package (WP)</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Functional Area (FA)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> - Work Package (WP)</t>
+    </r>
   </si>
   <si>
     <t>Role</t>
@@ -37,7 +59,13 @@
     <t>Velocity = 65%</t>
   </si>
   <si>
-    <t>per Functional Area [h]</t>
+    <t>per FA [h]</t>
+  </si>
+  <si>
+    <t>in days 1d = 8h</t>
+  </si>
+  <si>
+    <t>per FA [d]</t>
   </si>
   <si>
     <t>FA 1.1</t>
@@ -305,17 +333,56 @@
     <t>Analysis of evaluation feedback</t>
   </si>
   <si>
+    <t>FA 1.11</t>
+  </si>
+  <si>
+    <t>Project and Product Management</t>
+  </si>
+  <si>
+    <t>WP 1.11.1</t>
+  </si>
+  <si>
+    <t>Project Management, Ideation, Solution Design 1</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>WP 1.11.2</t>
+  </si>
+  <si>
+    <t>Project Management, Ideation, Solution Design 2</t>
+  </si>
+  <si>
+    <t>WP 1.11.3</t>
+  </si>
+  <si>
+    <t>Project Management, Ideation, Solution Design 3</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>estimated work hours</t>
+    <t>zur Orientierung Total SWS der LV über 3 Semester pro Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 SWS mal 4 (Wochen) mal 4 (Monate) mal 3 (Semester) </t>
+  </si>
+  <si>
+    <t>mal 3 Personen</t>
+  </si>
+  <si>
+    <t>SWS werden nicht ausreichen, um das Projekt fertigzustellen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###0.0"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -334,20 +401,29 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -364,7 +440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border/>
     <border>
       <bottom style="double">
@@ -381,11 +457,53 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF6D9EEB"/>
+      </left>
+      <top style="thick">
+        <color rgb="FF6D9EEB"/>
+      </top>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="FF6D9EEB"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF6D9EEB"/>
+      </top>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF6D9EEB"/>
+      </left>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="FF6D9EEB"/>
+      </right>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF6D9EEB"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FF6D9EEB"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thick">
+        <color rgb="FF6D9EEB"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="FF6D9EEB"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -396,13 +514,13 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -411,20 +529,38 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -645,17 +781,21 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="10.29"/>
-    <col customWidth="1" min="2" max="2" width="67.57"/>
-    <col customWidth="1" min="3" max="3" width="16.57"/>
-    <col customWidth="1" min="4" max="4" width="9.57"/>
-    <col customWidth="1" min="5" max="5" width="8.71"/>
-    <col customWidth="1" min="6" max="6" width="10.29"/>
-    <col customWidth="1" min="7" max="7" width="14.86"/>
-    <col customWidth="1" min="8" max="8" width="22.29"/>
+    <col customWidth="1" min="2" max="2" width="56.29"/>
+    <col customWidth="1" min="3" max="3" width="15.43"/>
+    <col customWidth="1" min="4" max="4" width="8.14"/>
+    <col customWidth="1" min="5" max="5" width="7.43"/>
+    <col customWidth="1" min="6" max="6" width="9.29"/>
+    <col customWidth="1" min="7" max="7" width="13.71"/>
+    <col customWidth="1" min="8" max="8" width="9.57"/>
+    <col customWidth="1" min="9" max="9" width="14.0"/>
+    <col customWidth="1" min="10" max="10" width="9.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1">
+        <v>2.0231208E7</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -664,7 +804,8 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -673,31 +814,37 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>8</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -705,46 +852,51 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="10">
+        <v>15</v>
+      </c>
+      <c r="D4" s="9">
         <v>3.0</v>
       </c>
       <c r="E4" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ref="F4:F7" si="1">SUM(D4*E4)</f>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" ref="G4:G7" si="2">SUM(F4*1.65)</f>
-        <v>49.5</v>
+        <v>39.6</v>
+      </c>
+      <c r="I4" s="11">
+        <f t="shared" ref="I4:I7" si="3">ROUND(G4 / 8, 1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>1000.0</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>0.025</v>
       </c>
       <c r="F5" s="9">
@@ -755,618 +907,731 @@
         <f t="shared" si="2"/>
         <v>41.25</v>
       </c>
+      <c r="I5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.2</v>
+      </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="10">
+        <v>15</v>
+      </c>
+      <c r="D6" s="9">
         <v>2.0</v>
       </c>
       <c r="E6" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="2"/>
-        <v>16.5</v>
+        <v>13.2</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" si="3"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="10">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9">
         <v>2.0</v>
       </c>
       <c r="E7" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>26.4</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="3"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="3"/>
       <c r="H8" s="3">
         <f>SUM(G4:G7)</f>
-        <v>140.25</v>
+        <v>120.45</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="3">
+        <f>ROUND(H8 / 8, 1)</f>
+        <v>15.1</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="10">
+        <v>26</v>
+      </c>
+      <c r="D9" s="9">
         <v>1.0</v>
       </c>
       <c r="E9" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" ref="F9:F11" si="3">SUM(D9*E9)</f>
-        <v>10</v>
+        <f t="shared" ref="F9:F11" si="4">SUM(D9*E9)</f>
+        <v>8</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" ref="G9:G11" si="4">SUM(F9*1.65)</f>
-        <v>16.5</v>
+        <f t="shared" ref="G9:G11" si="5">SUM(F9*1.65)</f>
+        <v>13.2</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" ref="I9:I11" si="6">ROUND(G9 / 8, 1)</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="10">
+        <v>15</v>
+      </c>
+      <c r="D10" s="9">
         <v>2.0</v>
       </c>
       <c r="E10" s="10">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="3"/>
-        <v>40</v>
+        <f t="shared" si="4"/>
+        <v>32</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" si="4"/>
-        <v>66</v>
+        <f t="shared" si="5"/>
+        <v>52.8</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="6"/>
+        <v>6.6</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="10">
+        <v>15</v>
+      </c>
+      <c r="D11" s="9">
         <v>2.0</v>
       </c>
       <c r="E11" s="10">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" si="3"/>
-        <v>40</v>
+        <f t="shared" si="4"/>
+        <v>32</v>
       </c>
       <c r="G11" s="9">
-        <f t="shared" si="4"/>
-        <v>66</v>
+        <f t="shared" si="5"/>
+        <v>52.8</v>
+      </c>
+      <c r="I11" s="11">
+        <f t="shared" si="6"/>
+        <v>6.6</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="3"/>
       <c r="H12" s="3">
         <f>SUM(G9:G11)</f>
-        <v>148.5</v>
+        <v>118.8</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="3">
+        <f>ROUND(H12 / 8, 1)</f>
+        <v>14.9</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="10">
+        <v>26</v>
+      </c>
+      <c r="D13" s="9">
         <v>3.0</v>
       </c>
       <c r="E13" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="F13" s="9">
         <f>SUM(D13*E13)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G13" s="9">
         <f>SUM(F13*1.65)</f>
-        <v>24.75</v>
+        <v>19.8</v>
+      </c>
+      <c r="I13" s="11">
+        <f>ROUND(G13 / 8, 1)</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="11"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="3"/>
       <c r="H14" s="3">
         <f>SUM(G13)</f>
-        <v>24.75</v>
+        <v>19.8</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="3">
+        <f>ROUND(H14 / 8, 1)</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="9">
         <v>1.0</v>
       </c>
       <c r="E15" s="10">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" ref="F15:F17" si="5">SUM(D15*E15)</f>
-        <v>10</v>
+        <f t="shared" ref="F15:F17" si="7">SUM(D15*E15)</f>
+        <v>4</v>
       </c>
       <c r="G15" s="9">
-        <f t="shared" ref="G15:G17" si="6">SUM(F15*1.65)</f>
-        <v>16.5</v>
+        <f t="shared" ref="G15:G17" si="8">SUM(F15*1.65)</f>
+        <v>6.6</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" ref="I15:I17" si="9">ROUND(G15 / 8, 1)</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="10">
+        <v>15</v>
+      </c>
+      <c r="D16" s="9">
         <v>2.0</v>
       </c>
       <c r="E16" s="10">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" si="5"/>
-        <v>20</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="G16" s="9">
-        <f t="shared" si="6"/>
-        <v>33</v>
+        <f t="shared" si="8"/>
+        <v>13.2</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="9"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>40</v>
+      <c r="A17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="12">
+        <v>15</v>
+      </c>
+      <c r="D17" s="13">
         <v>1.0</v>
       </c>
-      <c r="E17" s="12">
-        <v>20.0</v>
+      <c r="E17" s="14">
+        <v>16.0</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="5"/>
-        <v>20</v>
+        <f t="shared" si="7"/>
+        <v>16</v>
       </c>
       <c r="G17" s="9">
-        <f t="shared" si="6"/>
-        <v>33</v>
+        <f t="shared" si="8"/>
+        <v>26.4</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="9"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="3"/>
       <c r="H18" s="3">
         <f>SUM(G15:G17)</f>
-        <v>82.5</v>
+        <v>46.2</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="3">
+        <f>ROUND(H18 / 8, 1)</f>
+        <v>5.8</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D19" s="9">
         <v>1.0</v>
       </c>
       <c r="E19" s="10">
-        <v>10.0</v>
+        <v>4.0</v>
       </c>
       <c r="F19" s="9">
-        <f t="shared" ref="F19:F23" si="7">SUM(D19*E19)</f>
-        <v>10</v>
+        <f t="shared" ref="F19:F23" si="10">SUM(D19*E19)</f>
+        <v>4</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" ref="G19:G23" si="8">SUM(F19*1.65)</f>
-        <v>16.5</v>
+        <f t="shared" ref="G19:G23" si="11">SUM(F19*1.65)</f>
+        <v>6.6</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" ref="I19:I23" si="12">ROUND(G19 / 8, 1)</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>47</v>
+      <c r="A20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="12">
+        <v>26</v>
+      </c>
+      <c r="D20" s="13">
         <v>1.0</v>
       </c>
-      <c r="E20" s="12">
-        <v>10.0</v>
+      <c r="E20" s="14">
+        <v>8.0</v>
       </c>
       <c r="F20" s="9">
-        <f t="shared" si="7"/>
-        <v>10</v>
+        <f t="shared" si="10"/>
+        <v>8</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" si="8"/>
-        <v>16.5</v>
+        <f t="shared" si="11"/>
+        <v>13.2</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" si="12"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>49</v>
+      <c r="A21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="12">
+        <v>15</v>
+      </c>
+      <c r="D21" s="13">
         <v>2.0</v>
       </c>
-      <c r="E21" s="12">
-        <v>10.0</v>
+      <c r="E21" s="14">
+        <v>8.0</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" si="7"/>
-        <v>20</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" si="8"/>
-        <v>33</v>
+        <f t="shared" si="11"/>
+        <v>26.4</v>
+      </c>
+      <c r="I21" s="11">
+        <f t="shared" si="12"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>51</v>
+      <c r="A22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="12">
+        <v>15</v>
+      </c>
+      <c r="D22" s="13">
         <v>1.0</v>
       </c>
-      <c r="E22" s="12">
-        <v>20.0</v>
+      <c r="E22" s="14">
+        <v>16.0</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="7"/>
-        <v>20</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" si="8"/>
-        <v>33</v>
+        <f t="shared" si="11"/>
+        <v>26.4</v>
+      </c>
+      <c r="I22" s="11">
+        <f t="shared" si="12"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>53</v>
+      <c r="A23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="12">
+        <v>15</v>
+      </c>
+      <c r="D23" s="13">
         <v>1.0</v>
       </c>
-      <c r="E23" s="12">
-        <v>5.0</v>
+      <c r="E23" s="14">
+        <v>4.0</v>
       </c>
       <c r="F23" s="9">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" si="8"/>
-        <v>8.25</v>
+        <f t="shared" si="11"/>
+        <v>6.6</v>
+      </c>
+      <c r="I23" s="11">
+        <f t="shared" si="12"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+        <v>57</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="3"/>
       <c r="H24" s="3">
         <f>SUM(G19:G23)</f>
-        <v>107.25</v>
+        <v>79.2</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="3">
+        <f>ROUND(H24 / 8, 1)</f>
+        <v>9.9</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D25" s="10">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E25" s="10">
         <v>1.0</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" ref="F25:F31" si="9">SUM(D25*E25)</f>
-        <v>7</v>
+        <f t="shared" ref="F25:F31" si="13">SUM(D25*E25)</f>
+        <v>8</v>
       </c>
       <c r="G25" s="9">
-        <f t="shared" ref="G25:G31" si="10">SUM(F25*1.65)</f>
-        <v>11.55</v>
+        <f t="shared" ref="G25:G31" si="14">SUM(F25*1.65)</f>
+        <v>13.2</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" ref="I25:I31" si="15">ROUND(G25 / 8, 1)</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D26" s="10">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E26" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" si="9"/>
-        <v>3</v>
+        <f t="shared" si="13"/>
+        <v>8</v>
       </c>
       <c r="G26" s="9">
-        <f t="shared" si="10"/>
-        <v>4.95</v>
+        <f t="shared" si="14"/>
+        <v>13.2</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="15"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="10">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E27" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F27" s="9">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="G27" s="9">
-        <f t="shared" si="10"/>
-        <v>11.55</v>
+        <f t="shared" si="14"/>
+        <v>26.4</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" si="15"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D28" s="9">
         <v>1.0</v>
       </c>
       <c r="E28" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F28" s="9">
-        <f t="shared" si="9"/>
-        <v>10</v>
+        <f t="shared" si="13"/>
+        <v>8</v>
       </c>
       <c r="G28" s="9">
-        <f t="shared" si="10"/>
-        <v>16.5</v>
+        <f t="shared" si="14"/>
+        <v>13.2</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" si="15"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="10">
+        <v>15</v>
+      </c>
+      <c r="D29" s="9">
         <v>1.0</v>
       </c>
       <c r="E29" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F29" s="9">
-        <f t="shared" si="9"/>
-        <v>10</v>
+        <f t="shared" si="13"/>
+        <v>8</v>
       </c>
       <c r="G29" s="9">
-        <f t="shared" si="10"/>
-        <v>16.5</v>
+        <f t="shared" si="14"/>
+        <v>13.2</v>
+      </c>
+      <c r="I29" s="11">
+        <f t="shared" si="15"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="10">
+        <v>15</v>
+      </c>
+      <c r="D30" s="9">
         <v>2.0</v>
       </c>
       <c r="E30" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" si="9"/>
-        <v>20</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="G30" s="9">
-        <f t="shared" si="10"/>
-        <v>33</v>
+        <f t="shared" si="14"/>
+        <v>26.4</v>
+      </c>
+      <c r="I30" s="11">
+        <f t="shared" si="15"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="10">
+        <v>15</v>
+      </c>
+      <c r="D31" s="9">
         <v>1.0</v>
       </c>
       <c r="E31" s="10">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" si="9"/>
-        <v>20</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="G31" s="9">
-        <f t="shared" si="10"/>
-        <v>33</v>
+        <f t="shared" si="14"/>
+        <v>26.4</v>
+      </c>
+      <c r="I31" s="11">
+        <f t="shared" si="15"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1374,90 +1639,107 @@
       <c r="F32" s="3"/>
       <c r="H32" s="3">
         <f>SUM(G25:G31)</f>
-        <v>127.05</v>
+        <v>132</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="3">
+        <f>ROUND(H32 / 8, 1)</f>
+        <v>16.5</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>73</v>
+      <c r="A33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="10">
+        <v>15</v>
+      </c>
+      <c r="D33" s="9">
         <v>3.0</v>
       </c>
       <c r="E33" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" ref="F33:F35" si="11">SUM(D33*E33)</f>
+        <f t="shared" ref="F33:F35" si="16">SUM(D33*E33)</f>
+        <v>12</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" ref="G33:G35" si="17">SUM(F33*1.65)</f>
+        <v>19.8</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" ref="I33:I35" si="18">ROUND(G33 / 8, 1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="E34" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="F34" s="9">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="17"/>
+        <v>19.8</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" si="18"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="9">
-        <f t="shared" ref="G33:G35" si="12">SUM(F33*1.65)</f>
-        <v>24.75</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="10">
+      <c r="D35" s="9">
         <v>3.0</v>
       </c>
-      <c r="E34" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="F34" s="9">
-        <f t="shared" si="11"/>
-        <v>15</v>
-      </c>
-      <c r="G34" s="9">
-        <f t="shared" si="12"/>
-        <v>24.75</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="10">
-        <v>3.0</v>
-      </c>
       <c r="E35" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="F35" s="9">
-        <f t="shared" si="11"/>
-        <v>15</v>
+        <f t="shared" si="16"/>
+        <v>12</v>
       </c>
       <c r="G35" s="9">
-        <f t="shared" si="12"/>
-        <v>24.75</v>
+        <f t="shared" si="17"/>
+        <v>19.8</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="18"/>
+        <v>2.5</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1465,40 +1747,49 @@
       <c r="F36" s="3"/>
       <c r="H36" s="3">
         <f>SUM(G33:G35)</f>
-        <v>74.25</v>
+        <v>59.4</v>
+      </c>
+      <c r="I36" s="11"/>
+      <c r="J36" s="3">
+        <f>ROUND(H36 / 8, 1)</f>
+        <v>7.4</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>81</v>
+      <c r="A37" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="10">
+        <v>15</v>
+      </c>
+      <c r="D37" s="9">
         <v>2.0</v>
       </c>
       <c r="E37" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="F37" s="9">
         <f>SUM(D37*E37)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G37" s="9">
         <f>SUM(F37*1.65)</f>
-        <v>16.5</v>
+        <v>13.2</v>
+      </c>
+      <c r="I37" s="11">
+        <f>ROUND(G37 / 8, 1)</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1506,90 +1797,107 @@
       <c r="F38" s="3"/>
       <c r="H38" s="3">
         <f>SUM(G37)</f>
-        <v>16.5</v>
+        <v>13.2</v>
+      </c>
+      <c r="I38" s="11"/>
+      <c r="J38" s="3">
+        <f>ROUND(H38 / 8, 1)</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>85</v>
+      <c r="A39" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="10">
+        <v>26</v>
+      </c>
+      <c r="D39" s="9">
         <v>1.0</v>
       </c>
       <c r="E39" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F39" s="9">
-        <f t="shared" ref="F39:F41" si="13">SUM(D39*E39)</f>
-        <v>10</v>
+        <f t="shared" ref="F39:F41" si="19">SUM(D39*E39)</f>
+        <v>8</v>
       </c>
       <c r="G39" s="9">
-        <f t="shared" ref="G39:G41" si="14">SUM(F39*1.65)</f>
-        <v>16.5</v>
+        <f t="shared" ref="G39:G41" si="20">SUM(F39*1.65)</f>
+        <v>13.2</v>
+      </c>
+      <c r="I39" s="11">
+        <f t="shared" ref="I39:I41" si="21">ROUND(G39 / 8, 1)</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>87</v>
+      <c r="A40" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>89</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="10">
+        <v>26</v>
+      </c>
+      <c r="D40" s="9">
         <v>1.0</v>
       </c>
       <c r="E40" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F40" s="9">
-        <f t="shared" si="13"/>
-        <v>10</v>
+        <f t="shared" si="19"/>
+        <v>8</v>
       </c>
       <c r="G40" s="9">
-        <f t="shared" si="14"/>
-        <v>16.5</v>
+        <f t="shared" si="20"/>
+        <v>13.2</v>
+      </c>
+      <c r="I40" s="11">
+        <f t="shared" si="21"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>89</v>
+      <c r="A41" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="10">
+        <v>26</v>
+      </c>
+      <c r="D41" s="9">
         <v>1.0</v>
       </c>
       <c r="E41" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="F41" s="9">
-        <f t="shared" si="13"/>
-        <v>10</v>
+        <f t="shared" si="19"/>
+        <v>8</v>
       </c>
       <c r="G41" s="9">
-        <f t="shared" si="14"/>
-        <v>16.5</v>
+        <f t="shared" si="20"/>
+        <v>13.2</v>
+      </c>
+      <c r="I41" s="11">
+        <f t="shared" si="21"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>90</v>
+      <c r="A42" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1597,126 +1905,292 @@
       <c r="F42" s="3"/>
       <c r="H42" s="3">
         <f>SUM(G39:G41)</f>
-        <v>49.5</v>
+        <v>39.6</v>
+      </c>
+      <c r="I42" s="11"/>
+      <c r="J42" s="3">
+        <f>ROUND(H42 / 8, 1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>93</v>
+      <c r="A43" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="C43" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="E43" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="F43" s="9">
+        <f t="shared" ref="F43:F45" si="22">SUM(D43*E43)</f>
+        <v>12</v>
+      </c>
+      <c r="G43" s="9">
+        <f t="shared" ref="G43:G45" si="23">SUM(F43*1.65)</f>
+        <v>19.8</v>
+      </c>
+      <c r="I43" s="11">
+        <f t="shared" ref="I43:I45" si="24">ROUND(G43 / 8, 1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="9">
+        <v>6.0</v>
+      </c>
+      <c r="E44" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="F44" s="9">
+        <f t="shared" si="22"/>
         <v>24</v>
       </c>
-      <c r="D43" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="E43" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="F43" s="9">
-        <f t="shared" ref="F43:F45" si="15">SUM(D43*E43)</f>
-        <v>15</v>
-      </c>
-      <c r="G43" s="9">
-        <f t="shared" ref="G43:G45" si="16">SUM(F43*1.65)</f>
-        <v>24.75</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="E44" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="F44" s="9">
-        <f t="shared" si="15"/>
-        <v>30</v>
-      </c>
       <c r="G44" s="9">
-        <f t="shared" si="16"/>
-        <v>49.5</v>
+        <f t="shared" si="23"/>
+        <v>39.6</v>
+      </c>
+      <c r="I44" s="11">
+        <f t="shared" si="24"/>
+        <v>5</v>
       </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>96</v>
+      <c r="A45" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>98</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D45" s="9">
         <v>3.0</v>
       </c>
       <c r="E45" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" si="15"/>
-        <v>15</v>
+        <f t="shared" si="22"/>
+        <v>12</v>
       </c>
       <c r="G45" s="9">
-        <f t="shared" si="16"/>
-        <v>24.75</v>
+        <f t="shared" si="23"/>
+        <v>19.8</v>
+      </c>
+      <c r="I45" s="11">
+        <f t="shared" si="24"/>
+        <v>2.5</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="2"/>
+      <c r="A46" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="11">
+      <c r="H46" s="3">
         <f>SUM(G43:G45)</f>
-        <v>99</v>
+        <v>79.2</v>
+      </c>
+      <c r="I46" s="17"/>
+      <c r="J46" s="3">
+        <f>ROUND(H46 / 8, 1)</f>
+        <v>9.9</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16">
-        <f>SUM(F3:F38)</f>
-        <v>437</v>
-      </c>
-      <c r="G47" s="16">
-        <f>SUM(G3:G45)</f>
-        <v>869.55</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
+      <c r="A47" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="E47" s="10">
+        <v>64.0</v>
+      </c>
+      <c r="F47" s="9">
+        <f t="shared" ref="F47:F49" si="25">SUM(D47*E47)</f>
+        <v>192</v>
+      </c>
+      <c r="G47" s="9">
+        <f t="shared" ref="G47:G49" si="26">SUM(F47*1.65)</f>
+        <v>316.8</v>
+      </c>
+      <c r="I47" s="11">
+        <f t="shared" ref="I47:I49" si="27">ROUND(G47 / 8, 1)</f>
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="E48" s="10">
+        <v>16.0</v>
+      </c>
+      <c r="F48" s="9">
+        <f t="shared" si="25"/>
+        <v>48</v>
+      </c>
+      <c r="G48" s="9">
+        <f t="shared" si="26"/>
+        <v>79.2</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="11">
+        <f t="shared" si="27"/>
+        <v>9.9</v>
+      </c>
+      <c r="J48" s="9"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="E49" s="10">
+        <v>16.0</v>
+      </c>
+      <c r="F49" s="9">
+        <f t="shared" si="25"/>
+        <v>48</v>
+      </c>
+      <c r="G49" s="9">
+        <f t="shared" si="26"/>
+        <v>79.2</v>
+      </c>
+      <c r="H49" s="9"/>
+      <c r="I49" s="11">
+        <f t="shared" si="27"/>
+        <v>9.9</v>
+      </c>
+      <c r="J49" s="9"/>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="10"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3">
+        <f>SUM(G47:G49)</f>
+        <v>475.2</v>
+      </c>
+      <c r="I50" s="11"/>
+      <c r="J50" s="3">
+        <f>ROUND(H50 / 8, 1)</f>
+        <v>59.4</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="A51" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19">
+        <f t="shared" ref="F51:J51" si="28">SUM(F3:F50)</f>
+        <v>717</v>
+      </c>
+      <c r="G51" s="19">
+        <f t="shared" si="28"/>
+        <v>1183.05</v>
+      </c>
+      <c r="H51" s="19">
+        <f t="shared" si="28"/>
+        <v>1183.05</v>
+      </c>
+      <c r="I51" s="19">
+        <f t="shared" si="28"/>
+        <v>148.7</v>
+      </c>
+      <c r="J51" s="19">
+        <f t="shared" si="28"/>
+        <v>148.1</v>
+      </c>
+    </row>
     <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="B53" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="B54" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="23">
+        <f>4*4*4*3</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="B55" s="22"/>
+      <c r="C55" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="B56" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="26">
+        <f>C54*3</f>
+        <v>576</v>
+      </c>
+    </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1"/>
@@ -2411,6 +2885,260 @@
     <row r="748" ht="15.75" customHeight="1"/>
     <row r="749" ht="15.75" customHeight="1"/>
     <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>